<commit_message>
Various bang/bang control files
</commit_message>
<xml_diff>
--- a/Applications/Arduino/Simulink/TemperatureControl/Step03_BangBang/BangBangRunIDs.xlsx
+++ b/Applications/Arduino/Simulink/TemperatureControl/Step03_BangBang/BangBangRunIDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\MatlabLum\Applications\Arduino\Simulink\TemperatureControl\Step03_BangBang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F7D67B-F993-45C6-9834-6740BE606588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373DA7D8-87C6-4879-82D9-42835F853749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26460" yWindow="-16500" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="-14910" windowWidth="22455" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="36">
   <si>
     <t>File</t>
   </si>
@@ -94,6 +94,45 @@
   </si>
   <si>
     <t>no fan, shows chattering</t>
+  </si>
+  <si>
+    <t>deadbandSize_C</t>
+  </si>
+  <si>
+    <t>N/A only normal bang/bang</t>
+  </si>
+  <si>
+    <t>BangBangHysteresisSimulinkData_ID01</t>
+  </si>
+  <si>
+    <t>w/ hysteresis band, moving T_cmd</t>
+  </si>
+  <si>
+    <t>constant T_cmd</t>
+  </si>
+  <si>
+    <t>BangBangHysteresisSimulinkData_ID02</t>
+  </si>
+  <si>
+    <t>BangBangHysteresisSimulinkData_ID03</t>
+  </si>
+  <si>
+    <t>BangBangHysteresisSimulinkData_ID04</t>
+  </si>
+  <si>
+    <t>BangBangHysteresisSimulinkData_ID05</t>
+  </si>
+  <si>
+    <t>still no chatter</t>
+  </si>
+  <si>
+    <t>BangBangHysteresisSimulinkData_ID06</t>
+  </si>
+  <si>
+    <t>BangBangHysteresisSimulinkData_ID07</t>
+  </si>
+  <si>
+    <t>BangBangHysteresisSimulinkData_ID08</t>
   </si>
 </sst>
 </file>
@@ -146,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -158,7 +197,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,22 +477,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I10" sqref="A10:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="4"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="4"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,16 +509,19 @@
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -497,16 +538,19 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>45668</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -523,16 +567,19 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>45669</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -551,15 +598,18 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
@@ -577,15 +627,18 @@
       <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="4">
         <v>45680</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
@@ -603,12 +656,15 @@
       <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
@@ -626,12 +682,15 @@
       <c r="F7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
@@ -649,12 +708,15 @@
       <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
@@ -672,7 +734,230 @@
       <c r="F9" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="4">
+        <v>45689</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>120</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>45</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13">
+        <v>0.5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>0.2</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>0.05</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16">
+        <v>0.02</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17">
+        <v>0.01</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>